<commit_message>
Chaanges for sub to PLOS ONE: refs, figures and styling.
</commit_message>
<xml_diff>
--- a/CRediT.xlsx
+++ b/CRediT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\TEMPOSR-A1953\TEMPO_syst-rev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\TEMPOSR-A1953\TEMPO_syst-rev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>#</t>
   </si>
@@ -452,7 +452,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,6 +492,9 @@
       <c r="C2" t="s">
         <v>34</v>
       </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
       <c r="E2" t="s">
         <v>35</v>
       </c>
@@ -523,6 +526,9 @@
       <c r="C4" t="s">
         <v>34</v>
       </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
@@ -534,6 +540,9 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
@@ -576,6 +585,9 @@
       <c r="C8" t="s">
         <v>34</v>
       </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" t="s">
         <v>35</v>
       </c>
@@ -593,6 +605,9 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
@@ -618,6 +633,9 @@
       <c r="B11" t="s">
         <v>26</v>
       </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" t="s">
         <v>35</v>
       </c>
@@ -675,6 +693,9 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
         <v>34</v>
       </c>
       <c r="E15" t="s">

</xml_diff>